<commit_message>
Added justification, image, audio attributes in respect for the corresponding data mapping
</commit_message>
<xml_diff>
--- a/public/resources/series-test/series-test.xlsx
+++ b/public/resources/series-test/series-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esayi\Documents\Data\Projects\j2hb-backend\public\resources\series-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE02B0EE-871E-4A37-A9C6-9CB6910F1C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4632BE2F-F59B-4270-877F-980F443DA4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Correction</t>
   </si>
@@ -78,6 +78,30 @@
     <t>Reponse 4</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/0ja037rb12ct9zrk9bod1/1.png?rlkey=bfa2xbsm386gw8pc6c32pvc5r&amp;dl=0</t>
+  </si>
+  <si>
+    <t>https://www2.cs.uic.edu/~i101/SoundFiles/taunt.wav</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/hcciyeycemphpedsqq84v/Screenshot-2024-01-29-at-18.52.22.png?rlkey=8pio49940zj7xfvn8f3d1x36h&amp;dl=0</t>
+  </si>
+  <si>
+    <t>Justification</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
     <t>700 دَرْهَمْ</t>
   </si>
 </sst>
@@ -85,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +131,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -139,40 +171,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Head" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,100 +537,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="20.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="48" style="3" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="54.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="127.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="20.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J1"/>
-      <c r="K1"/>
-    </row>
-    <row r="2" spans="1:12" ht="36" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J2"/>
-      <c r="K2"/>
-    </row>
-    <row r="3" spans="1:12" ht="54" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="J2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4">
+      <c r="E3" s="12"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12">
         <v>2</v>
       </c>
-      <c r="J3"/>
-      <c r="K3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -560,7 +670,7 @@
       <c r="K4"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -574,7 +684,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -588,7 +698,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -602,7 +712,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -616,7 +726,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -630,7 +740,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -644,7 +754,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -658,7 +768,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -672,7 +782,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -686,7 +796,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -700,7 +810,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -714,7 +824,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -728,7 +838,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -742,7 +852,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -756,7 +866,7 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -770,7 +880,7 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -784,7 +894,7 @@
       <c r="K20"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -798,7 +908,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -812,7 +922,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -826,7 +936,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -840,7 +950,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -854,7 +964,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -868,7 +978,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -882,7 +992,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -896,7 +1006,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -910,7 +1020,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -924,7 +1034,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -938,7 +1048,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -952,7 +1062,7 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -966,7 +1076,7 @@
       <c r="K33"/>
       <c r="L33"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -980,7 +1090,7 @@
       <c r="K34"/>
       <c r="L34"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -994,7 +1104,7 @@
       <c r="K35"/>
       <c r="L35"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -1008,7 +1118,7 @@
       <c r="K36"/>
       <c r="L36"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -1022,7 +1132,7 @@
       <c r="K37"/>
       <c r="L37"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -1036,7 +1146,7 @@
       <c r="K38"/>
       <c r="L38"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -1050,7 +1160,7 @@
       <c r="K39"/>
       <c r="L39"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -1064,7 +1174,7 @@
       <c r="K40"/>
       <c r="L40"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -1078,7 +1188,7 @@
       <c r="K41"/>
       <c r="L41"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -1092,7 +1202,7 @@
       <c r="K42"/>
       <c r="L42"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -1106,7 +1216,7 @@
       <c r="K43"/>
       <c r="L43"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -1120,7 +1230,7 @@
       <c r="K44"/>
       <c r="L44"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -1134,7 +1244,7 @@
       <c r="K45"/>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -1148,7 +1258,7 @@
       <c r="K46"/>
       <c r="L46"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -1162,7 +1272,7 @@
       <c r="K47"/>
       <c r="L47"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -1176,7 +1286,7 @@
       <c r="K48"/>
       <c r="L48"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -1190,7 +1300,7 @@
       <c r="K49"/>
       <c r="L49"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -1204,7 +1314,7 @@
       <c r="K50"/>
       <c r="L50"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -1218,7 +1328,7 @@
       <c r="K51"/>
       <c r="L51"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -1232,7 +1342,7 @@
       <c r="K52"/>
       <c r="L52"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -1246,7 +1356,7 @@
       <c r="K53"/>
       <c r="L53"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -1260,7 +1370,7 @@
       <c r="K54"/>
       <c r="L54"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -1274,7 +1384,7 @@
       <c r="K55"/>
       <c r="L55"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -1288,7 +1398,7 @@
       <c r="K56"/>
       <c r="L56"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -1302,7 +1412,7 @@
       <c r="K57"/>
       <c r="L57"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -1316,7 +1426,7 @@
       <c r="K58"/>
       <c r="L58"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -1330,7 +1440,7 @@
       <c r="K59"/>
       <c r="L59"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -1344,7 +1454,7 @@
       <c r="K60"/>
       <c r="L60"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -1358,7 +1468,7 @@
       <c r="K61"/>
       <c r="L61"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -1372,7 +1482,7 @@
       <c r="K62"/>
       <c r="L62"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -1386,7 +1496,7 @@
       <c r="K63"/>
       <c r="L63"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -1400,7 +1510,7 @@
       <c r="K64"/>
       <c r="L64"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -1414,7 +1524,7 @@
       <c r="K65"/>
       <c r="L65"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -1428,7 +1538,7 @@
       <c r="K66"/>
       <c r="L66"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -1442,7 +1552,7 @@
       <c r="K67"/>
       <c r="L67"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -1456,7 +1566,7 @@
       <c r="K68"/>
       <c r="L68"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -1470,7 +1580,7 @@
       <c r="K69"/>
       <c r="L69"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -1484,7 +1594,7 @@
       <c r="K70"/>
       <c r="L70"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -1498,7 +1608,7 @@
       <c r="K71"/>
       <c r="L71"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -1512,7 +1622,7 @@
       <c r="K72"/>
       <c r="L72"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -1526,7 +1636,7 @@
       <c r="K73"/>
       <c r="L73"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -1540,7 +1650,7 @@
       <c r="K74"/>
       <c r="L74"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -1554,7 +1664,7 @@
       <c r="K75"/>
       <c r="L75"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -1568,7 +1678,7 @@
       <c r="K76"/>
       <c r="L76"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -1582,7 +1692,7 @@
       <c r="K77"/>
       <c r="L77"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -1596,7 +1706,7 @@
       <c r="K78"/>
       <c r="L78"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -1610,7 +1720,7 @@
       <c r="K79"/>
       <c r="L79"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -1624,7 +1734,7 @@
       <c r="K80"/>
       <c r="L80"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -1638,7 +1748,7 @@
       <c r="K81"/>
       <c r="L81"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -1652,7 +1762,7 @@
       <c r="K82"/>
       <c r="L82"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -1666,7 +1776,7 @@
       <c r="K83"/>
       <c r="L83"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -1680,7 +1790,7 @@
       <c r="K84"/>
       <c r="L84"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -1694,7 +1804,7 @@
       <c r="K85"/>
       <c r="L85"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -1708,7 +1818,7 @@
       <c r="K86"/>
       <c r="L86"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -1722,7 +1832,7 @@
       <c r="K87"/>
       <c r="L87"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -1736,7 +1846,7 @@
       <c r="K88"/>
       <c r="L88"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -1750,7 +1860,7 @@
       <c r="K89"/>
       <c r="L89"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -1764,7 +1874,7 @@
       <c r="K90"/>
       <c r="L90"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -1778,7 +1888,7 @@
       <c r="K91"/>
       <c r="L91"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -1792,7 +1902,7 @@
       <c r="K92"/>
       <c r="L92"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -1806,7 +1916,7 @@
       <c r="K93"/>
       <c r="L93"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -1820,7 +1930,7 @@
       <c r="K94"/>
       <c r="L94"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -1834,7 +1944,7 @@
       <c r="K95"/>
       <c r="L95"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -1848,7 +1958,7 @@
       <c r="K96"/>
       <c r="L96"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -1862,7 +1972,7 @@
       <c r="K97"/>
       <c r="L97"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -1876,7 +1986,7 @@
       <c r="K98"/>
       <c r="L98"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -1890,7 +2000,7 @@
       <c r="K99"/>
       <c r="L99"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -1904,7 +2014,7 @@
       <c r="K100"/>
       <c r="L100"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -1918,7 +2028,7 @@
       <c r="K101"/>
       <c r="L101"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -1932,7 +2042,7 @@
       <c r="K102"/>
       <c r="L102"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -1946,7 +2056,7 @@
       <c r="K103"/>
       <c r="L103"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -1960,7 +2070,7 @@
       <c r="K104"/>
       <c r="L104"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -1974,7 +2084,7 @@
       <c r="K105"/>
       <c r="L105"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -1988,7 +2098,7 @@
       <c r="K106"/>
       <c r="L106"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -2002,7 +2112,7 @@
       <c r="K107"/>
       <c r="L107"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -2016,7 +2126,7 @@
       <c r="K108"/>
       <c r="L108"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -2030,7 +2140,7 @@
       <c r="K109"/>
       <c r="L109"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -2044,7 +2154,7 @@
       <c r="K110"/>
       <c r="L110"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -2058,7 +2168,7 @@
       <c r="K111"/>
       <c r="L111"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -2072,7 +2182,7 @@
       <c r="K112"/>
       <c r="L112"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
@@ -2086,7 +2196,7 @@
       <c r="K113"/>
       <c r="L113"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -2100,7 +2210,7 @@
       <c r="K114"/>
       <c r="L114"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
@@ -2114,7 +2224,7 @@
       <c r="K115"/>
       <c r="L115"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -2128,7 +2238,7 @@
       <c r="K116"/>
       <c r="L116"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -2142,7 +2252,7 @@
       <c r="K117"/>
       <c r="L117"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -2156,7 +2266,7 @@
       <c r="K118"/>
       <c r="L118"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -2170,7 +2280,7 @@
       <c r="K119"/>
       <c r="L119"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -2184,7 +2294,7 @@
       <c r="K120"/>
       <c r="L120"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
@@ -2198,7 +2308,7 @@
       <c r="K121"/>
       <c r="L121"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
@@ -2212,7 +2322,7 @@
       <c r="K122"/>
       <c r="L122"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -2226,7 +2336,7 @@
       <c r="K123"/>
       <c r="L123"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
@@ -2240,7 +2350,7 @@
       <c r="K124"/>
       <c r="L124"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
@@ -2254,7 +2364,7 @@
       <c r="K125"/>
       <c r="L125"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
@@ -2268,7 +2378,7 @@
       <c r="K126"/>
       <c r="L126"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -2282,7 +2392,7 @@
       <c r="K127"/>
       <c r="L127"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
@@ -2296,7 +2406,7 @@
       <c r="K128"/>
       <c r="L128"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
@@ -2310,7 +2420,7 @@
       <c r="K129"/>
       <c r="L129"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -2324,7 +2434,7 @@
       <c r="K130"/>
       <c r="L130"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -2338,7 +2448,7 @@
       <c r="K131"/>
       <c r="L131"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -2352,7 +2462,7 @@
       <c r="K132"/>
       <c r="L132"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
@@ -2366,7 +2476,7 @@
       <c r="K133"/>
       <c r="L133"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -2380,7 +2490,7 @@
       <c r="K134"/>
       <c r="L134"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -2394,7 +2504,7 @@
       <c r="K135"/>
       <c r="L135"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136"/>
       <c r="B136"/>
       <c r="C136"/>
@@ -2408,7 +2518,7 @@
       <c r="K136"/>
       <c r="L136"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137"/>
       <c r="B137"/>
       <c r="C137"/>
@@ -2422,7 +2532,7 @@
       <c r="K137"/>
       <c r="L137"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -2436,7 +2546,7 @@
       <c r="K138"/>
       <c r="L138"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139"/>
       <c r="B139"/>
       <c r="C139"/>
@@ -2450,7 +2560,7 @@
       <c r="K139"/>
       <c r="L139"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140"/>
       <c r="B140"/>
       <c r="C140"/>
@@ -2464,7 +2574,7 @@
       <c r="K140"/>
       <c r="L140"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141"/>
       <c r="B141"/>
       <c r="C141"/>
@@ -2478,7 +2588,7 @@
       <c r="K141"/>
       <c r="L141"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142"/>
       <c r="B142"/>
       <c r="C142"/>
@@ -2492,7 +2602,7 @@
       <c r="K142"/>
       <c r="L142"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143"/>
       <c r="B143"/>
       <c r="C143"/>
@@ -2506,7 +2616,7 @@
       <c r="K143"/>
       <c r="L143"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144"/>
       <c r="B144"/>
       <c r="C144"/>
@@ -2520,7 +2630,7 @@
       <c r="K144"/>
       <c r="L144"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145"/>
       <c r="B145"/>
       <c r="C145"/>
@@ -2534,7 +2644,7 @@
       <c r="K145"/>
       <c r="L145"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146"/>
       <c r="B146"/>
       <c r="C146"/>
@@ -2548,7 +2658,7 @@
       <c r="K146"/>
       <c r="L146"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147"/>
       <c r="B147"/>
       <c r="C147"/>
@@ -2562,7 +2672,7 @@
       <c r="K147"/>
       <c r="L147"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148"/>
       <c r="B148"/>
       <c r="C148"/>
@@ -2576,7 +2686,7 @@
       <c r="K148"/>
       <c r="L148"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149"/>
       <c r="B149"/>
       <c r="C149"/>
@@ -2590,7 +2700,7 @@
       <c r="K149"/>
       <c r="L149"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150"/>
       <c r="B150"/>
       <c r="C150"/>
@@ -2604,7 +2714,7 @@
       <c r="K150"/>
       <c r="L150"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151"/>
       <c r="B151"/>
       <c r="C151"/>
@@ -2618,7 +2728,7 @@
       <c r="K151"/>
       <c r="L151"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152"/>
       <c r="B152"/>
       <c r="C152"/>
@@ -2632,7 +2742,7 @@
       <c r="K152"/>
       <c r="L152"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153"/>
       <c r="B153"/>
       <c r="C153"/>
@@ -2646,7 +2756,7 @@
       <c r="K153"/>
       <c r="L153"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154"/>
       <c r="B154"/>
       <c r="C154"/>
@@ -2661,7 +2771,11 @@
       <c r="L154"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{7A79E04C-D79E-4BFF-9D5D-7E205AC1F240}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{E9FA5CD4-9117-41BF-85E0-6C79B5724E0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>